<commit_message>
ajout du texte d'avertissement sous les champs du formulaire
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toons\Developpement\Cours Openclassrooms\Projet 05\Projet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A2B38B-CAF0-4333-9B26-367C177F450C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -43,26 +52,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Montserrat"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Montserrat"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <name val="Montserrat"/>
     </font>
   </fonts>
@@ -71,7 +80,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -81,7 +90,13 @@
     </fill>
   </fills>
   <borders count="17">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -95,8 +110,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -106,6 +123,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -120,6 +138,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -134,6 +153,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -142,17 +162,22 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -161,9 +186,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -172,9 +199,11 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -189,8 +218,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -200,6 +231,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -214,6 +246,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -228,6 +261,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -242,8 +276,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -253,6 +289,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -267,6 +304,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -281,92 +319,81 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -556,26 +583,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.29"/>
-    <col customWidth="1" min="2" max="3" width="58.43"/>
-    <col customWidth="1" min="4" max="4" width="57.86"/>
-    <col customWidth="1" min="5" max="5" width="52.71"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="3" width="58.44140625" customWidth="1"/>
+    <col min="4" max="4" width="57.88671875" customWidth="1"/>
+    <col min="5" max="5" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.5" customHeight="1">
+    <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -590,9 +622,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="64.8" x14ac:dyDescent="0.5">
       <c r="A2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -607,157 +639,157 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A3" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4">
-      <c r="A4" s="13">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="13" t="s">
+    <row r="4" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="17"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="17"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="17"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="17"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="17"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="17"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="17"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="17"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="17"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="17"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="17"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
plan de test complété
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toons\Developpement\Cours Openclassrooms\Projet 05\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A2B38B-CAF0-4333-9B26-367C177F450C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF29F560-0375-4AF3-B261-F3A984FE8C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -43,10 +43,43 @@
     <t>Affichage de l'ensemble des produits</t>
   </si>
   <si>
-    <t>OK / Description erreur</t>
-  </si>
-  <si>
-    <t>...</t>
+    <t>Une page “produit” qui affiche (de manière dynamique) les détails du produit sur
+lequel l'utilisateur a cliqué depuis la page d’accueil. Depuis cette page, l’utilisateur
+peut sélectionner une quantité, une couleur, et ajouter le produit à son panier.</t>
+  </si>
+  <si>
+    <t>Affichage d'un seul produit</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page produit du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>Une page “panier”. Celle-ci contient plusieurs parties :
+○ Un résumé des produits dans le panier, le prix total et la possibilité de
+modifier la quantité d’un produit sélectionné ou bien de supprimer celui-ci.
+○ Un formulaire permettant de passer une commande. Les données du
+formulaire doivent être correctes et bien formatées avant d'être renvoyées au
+back-end. Par exemple, pas de chiffre dans un champ prénom.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page panier du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>Affichage des produits ajouté au panier</t>
+  </si>
+  <si>
+    <t>Une page “confirmation” :
+○ Un message de confirmation de commande, remerciant l'utilisateur pour sa
+commande, et indiquant l'identifiant de commande envoyé par l’API.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page confirmation du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>Confirmation et affichage de son numéro de commande.</t>
   </si>
 </sst>
 </file>
@@ -325,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -348,9 +381,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -374,6 +404,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +632,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -635,161 +671,182 @@
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A3" s="9">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A4" s="9">
+      <c r="C3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="259.2" x14ac:dyDescent="0.5">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A5" s="9">
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="108" x14ac:dyDescent="0.5">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
+      <c r="B5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout de function et suppression d'alerte dans page cart.js
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toons\Developpement\Cours Openclassrooms\Projet 05\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF29F560-0375-4AF3-B261-F3A984FE8C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B523D0A-A4E5-4DEF-BFAB-A6C4F1E9C20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,29 +57,29 @@
     <t>Ouvrir sur la page produit du site web dans un navigateur</t>
   </si>
   <si>
+    <t>Ouvrir sur la page panier du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>Affichage des produits ajouté au panier</t>
+  </si>
+  <si>
+    <t>Une page “confirmation” :
+○ Un message de confirmation de commande, remerciant l'utilisateur pour sa
+commande, et indiquant l'identifiant de commande envoyé par l’API.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page confirmation du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>Confirmation et affichage de son numéro de commande.</t>
+  </si>
+  <si>
     <t>Une page “panier”. Celle-ci contient plusieurs parties :
 ○ Un résumé des produits dans le panier, le prix total et la possibilité de
 modifier la quantité d’un produit sélectionné ou bien de supprimer celui-ci.
 ○ Un formulaire permettant de passer une commande. Les données du
 formulaire doivent être correctes et bien formatées avant d'être renvoyées au
-back-end. Par exemple, pas de chiffre dans un champ prénom.</t>
-  </si>
-  <si>
-    <t>Ouvrir sur la page panier du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t>Affichage des produits ajouté au panier</t>
-  </si>
-  <si>
-    <t>Une page “confirmation” :
-○ Un message de confirmation de commande, remerciant l'utilisateur pour sa
-commande, et indiquant l'identifiant de commande envoyé par l’API.</t>
-  </si>
-  <si>
-    <t>Ouvrir sur la page confirmation du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t>Confirmation et affichage de son numéro de commande.</t>
+back-end.</t>
   </si>
 </sst>
 </file>
@@ -131,67 +131,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -202,7 +142,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -213,8 +155,94 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -230,7 +258,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -240,7 +268,7 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -254,6 +282,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -261,8 +319,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -276,8 +334,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -286,71 +344,13 @@
         <color rgb="FF000000"/>
       </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -358,58 +358,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,11 +625,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -643,7 +641,7 @@
     <col min="5" max="5" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -658,195 +656,77 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="64.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="5">
+    <row r="2" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="129.6" x14ac:dyDescent="0.5">
-      <c r="A3" s="8">
+    <row r="3" spans="1:5" ht="129.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="259.2" x14ac:dyDescent="0.5">
-      <c r="A4" s="8">
+    <row r="4" spans="1:5" ht="237.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="108.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="C5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="108" x14ac:dyDescent="0.5">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="62" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
amelioration du plan de test
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toons\Developpement\Cours Openclassrooms\Projet 05\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toons\Developpement\Cours Openclassrooms\Projet 05\Soutenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B523D0A-A4E5-4DEF-BFAB-A6C4F1E9C20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B415367-8BF9-4AC7-986A-2CD3D3189E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -43,43 +43,111 @@
     <t>Affichage de l'ensemble des produits</t>
   </si>
   <si>
-    <t>Une page “produit” qui affiche (de manière dynamique) les détails du produit sur
-lequel l'utilisateur a cliqué depuis la page d’accueil. Depuis cette page, l’utilisateur
-peut sélectionner une quantité, une couleur, et ajouter le produit à son panier.</t>
+    <t>Ouvrir sur la page produit du site web dans un navigateur</t>
   </si>
   <si>
     <t>Affichage d'un seul produit</t>
   </si>
   <si>
+    <t>Affichage de la couleur</t>
+  </si>
+  <si>
+    <t>Affichage de la quantité</t>
+  </si>
+  <si>
+    <t>Ajout au panier</t>
+  </si>
+  <si>
+    <t>Augmente ou baisse la quantité</t>
+  </si>
+  <si>
+    <t>Ouvre une liste déroulante</t>
+  </si>
+  <si>
+    <t>Affichage d'un pop-up de direction</t>
+  </si>
+  <si>
+    <t>Dans cette page produit, l’utilisateur
+peut sélectionner une couleur,</t>
+  </si>
+  <si>
+    <t>Dans cette page produit, l’utilisateur
+peut sélectionner une quantité.</t>
+  </si>
+  <si>
+    <t>Dans cette page produit, l’utilisateur peut ajouter le produit à son panier.</t>
+  </si>
+  <si>
+    <t>Dans cette page panier, l’utilisateur à la possibilité de supprimer celui-ci.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page panier du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>Affichage des produits ajouté au panier</t>
+  </si>
+  <si>
+    <t>Dans cette page panier, l’utilisateur à la possibilité de modifier la quantité d’un produit sélectionné.</t>
+  </si>
+  <si>
+    <t>Dans cette page panier. Contient un formulaire permettant de passer une commande.</t>
+  </si>
+  <si>
+    <t>Dans cette page panier, l’utilisateur peut passer la commande.</t>
+  </si>
+  <si>
+    <t>Suppression de l'article</t>
+  </si>
+  <si>
+    <t>Les données du
+formulaire doivent être correctes et bien formatées.</t>
+  </si>
+  <si>
+    <t>Champs dédiés aux utilisateurs</t>
+  </si>
+  <si>
+    <t>Article supprimé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Données de l'utilisateur </t>
+  </si>
+  <si>
+    <t>Données valide ou non</t>
+  </si>
+  <si>
+    <t>Affichage d'un message d'erreur si non valide</t>
+  </si>
+  <si>
+    <t>Commande effectuée</t>
+  </si>
+  <si>
+    <t>Commande passée</t>
+  </si>
+  <si>
+    <t>Une page produit qui affiche (de manière dynamique) les détails du produit sur
+lequel l'utilisateur a cliqué depuis la page d’accueil.</t>
+  </si>
+  <si>
+    <t>Une page panier. Celle-ci contient : le ou les articles ajouté, un résumé du ou des produits dans le panier, le nombre total d'article et le prix total.</t>
+  </si>
+  <si>
+    <t>Dans cette page confirmation, indique l'identifiant de commande envoyé par l’API.</t>
+  </si>
+  <si>
+    <t>Une page confirmation montrant un message de confirmation de commande, remerciant l'utilisateur pour sa
+commande.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page confirmation du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>Message de confirmation</t>
+  </si>
+  <si>
+    <t>Affichage du numéro de commande</t>
+  </si>
+  <si>
     <t>OK</t>
-  </si>
-  <si>
-    <t>Ouvrir sur la page produit du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t>Ouvrir sur la page panier du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t>Affichage des produits ajouté au panier</t>
-  </si>
-  <si>
-    <t>Une page “confirmation” :
-○ Un message de confirmation de commande, remerciant l'utilisateur pour sa
-commande, et indiquant l'identifiant de commande envoyé par l’API.</t>
-  </si>
-  <si>
-    <t>Ouvrir sur la page confirmation du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t>Confirmation et affichage de son numéro de commande.</t>
-  </si>
-  <si>
-    <t>Une page “panier”. Celle-ci contient plusieurs parties :
-○ Un résumé des produits dans le panier, le prix total et la possibilité de
-modifier la quantité d’un produit sélectionné ou bien de supprimer celui-ci.
-○ Un formulaire permettant de passer une commande. Les données du
-formulaire doivent être correctes et bien formatées avant d'être renvoyées au
-back-end.</t>
   </si>
 </sst>
 </file>
@@ -108,7 +176,7 @@
       <name val="Montserrat"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +189,12 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -358,8 +432,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -372,24 +459,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -399,13 +483,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -625,12 +724,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -638,95 +736,267 @@
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="3" width="58.44140625" customWidth="1"/>
     <col min="4" max="4" width="57.88671875" customWidth="1"/>
-    <col min="5" max="5" width="52.6640625" customWidth="1"/>
+    <col min="5" max="5" width="52.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="129.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="E5" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" ht="86.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E10" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <v>8</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="237.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>11</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:5" ht="86.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
         <v>12</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="108.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="65.400000000000006" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
         <v>13</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>9</v>
+      <c r="B17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="62" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modification du plan de test
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toons\Developpement\Cours Openclassrooms\Projet 05\Soutenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B415367-8BF9-4AC7-986A-2CD3D3189E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328A30F5-0EAD-4F6F-995D-3A3EB890B560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -43,28 +43,7 @@
     <t>Affichage de l'ensemble des produits</t>
   </si>
   <si>
-    <t>Ouvrir sur la page produit du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t>Affichage d'un seul produit</t>
-  </si>
-  <si>
-    <t>Affichage de la couleur</t>
-  </si>
-  <si>
     <t>Affichage de la quantité</t>
-  </si>
-  <si>
-    <t>Ajout au panier</t>
-  </si>
-  <si>
-    <t>Augmente ou baisse la quantité</t>
-  </si>
-  <si>
-    <t>Ouvre une liste déroulante</t>
-  </si>
-  <si>
-    <t>Affichage d'un pop-up de direction</t>
   </si>
   <si>
     <t>Dans cette page produit, l’utilisateur
@@ -75,53 +54,13 @@
 peut sélectionner une quantité.</t>
   </si>
   <si>
-    <t>Dans cette page produit, l’utilisateur peut ajouter le produit à son panier.</t>
-  </si>
-  <si>
     <t>Dans cette page panier, l’utilisateur à la possibilité de supprimer celui-ci.</t>
   </si>
   <si>
-    <t>Ouvrir sur la page panier du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t>Affichage des produits ajouté au panier</t>
-  </si>
-  <si>
     <t>Dans cette page panier, l’utilisateur à la possibilité de modifier la quantité d’un produit sélectionné.</t>
   </si>
   <si>
     <t>Dans cette page panier. Contient un formulaire permettant de passer une commande.</t>
-  </si>
-  <si>
-    <t>Dans cette page panier, l’utilisateur peut passer la commande.</t>
-  </si>
-  <si>
-    <t>Suppression de l'article</t>
-  </si>
-  <si>
-    <t>Les données du
-formulaire doivent être correctes et bien formatées.</t>
-  </si>
-  <si>
-    <t>Champs dédiés aux utilisateurs</t>
-  </si>
-  <si>
-    <t>Article supprimé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Données de l'utilisateur </t>
-  </si>
-  <si>
-    <t>Données valide ou non</t>
-  </si>
-  <si>
-    <t>Affichage d'un message d'erreur si non valide</t>
-  </si>
-  <si>
-    <t>Commande effectuée</t>
-  </si>
-  <si>
-    <t>Commande passée</t>
   </si>
   <si>
     <t>Une page produit qui affiche (de manière dynamique) les détails du produit sur
@@ -131,23 +70,100 @@
     <t>Une page panier. Celle-ci contient : le ou les articles ajouté, un résumé du ou des produits dans le panier, le nombre total d'article et le prix total.</t>
   </si>
   <si>
-    <t>Dans cette page confirmation, indique l'identifiant de commande envoyé par l’API.</t>
-  </si>
-  <si>
-    <t>Une page confirmation montrant un message de confirmation de commande, remerciant l'utilisateur pour sa
-commande.</t>
-  </si>
-  <si>
-    <t>Ouvrir sur la page confirmation du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t>Message de confirmation</t>
-  </si>
-  <si>
-    <t>Affichage du numéro de commande</t>
-  </si>
-  <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>Affichage du produit, avec ses caractéristiques affiché, dont le nom, le prix, la description, le choix de la couleur, la quantité et un bouton pour ajouter le produit au panier</t>
+  </si>
+  <si>
+    <t>Affichage des choix de couleus</t>
+  </si>
+  <si>
+    <t>Un pop-up s'affiche pour indiquer a l'utilisateur si il veut être rediriger dans son panier ou non</t>
+  </si>
+  <si>
+    <t>Affichage des produits ajouté au panier avec un petit résumer de ses caractéristique,  de la quantité choisi, le total d'articles et du prix suivi du formulaire  et du bouton commander</t>
+  </si>
+  <si>
+    <t>Affichage de la nouvelle quantité et du total modifié</t>
+  </si>
+  <si>
+    <t>L'article est supprimé du panier et le total est modifié</t>
+  </si>
+  <si>
+    <t>L'utilisateurs inscrit son nom, prénom, adresse, ville et email</t>
+  </si>
+  <si>
+    <t>Les coordonnées de l'utilisateur son affiché</t>
+  </si>
+  <si>
+    <t>Aucun message d'erreur s'affiche</t>
+  </si>
+  <si>
+    <t>Les données du formulaire sont correctes et bien formatées.</t>
+  </si>
+  <si>
+    <t>Les données du formulaire sont incorrectes et mal formatées.</t>
+  </si>
+  <si>
+    <t>L'utilisateur inscrit ses coordonnées qui sont valides</t>
+  </si>
+  <si>
+    <t>L'utilisateur inscrit ses coordonnées qui ne sont pas valides</t>
+  </si>
+  <si>
+    <t>Un message d'erreur s'affiche qui explique les conditions pour que ce soit valide</t>
+  </si>
+  <si>
+    <t>Clique sur le bouton pour modifié la quantité en augmentant ou en baissant</t>
+  </si>
+  <si>
+    <t>Clique sur OK dans le pop-up et la page panier du site web s'ouvre dans le navigateur</t>
+  </si>
+  <si>
+    <t>Clique sur les bouton pour augmenter ou baisser la quantité d'article choisi</t>
+  </si>
+  <si>
+    <t>Clique sur la liste des choix de couleur et une liste déroulante s'ouvre</t>
+  </si>
+  <si>
+    <t>Clique sur le produit selectionné depuis la page d’accueil et ouvre la page produit du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>l'utilisateur est redirigé vers la page confirmation</t>
+  </si>
+  <si>
+    <t>Une page de confirmation montrant un message de commande validée avec son numéro de commande unique.</t>
+  </si>
+  <si>
+    <t>Message de confirmation qui explique que la commande à bien était validée avec son numéro de commande unique inscrit</t>
+  </si>
+  <si>
+    <t>Dans cette page panier, l’utilisateur peut passer la commande avec le bouton dédié si ses coordonnées sont valides et avec au moins un article.</t>
+  </si>
+  <si>
+    <t>Clique sur le bouton commande avec au moins un article et le fomulaire bien rempli</t>
+  </si>
+  <si>
+    <t>Après le clique du bouton de commande la page de confirmation du site web s'ouvre dans le navigateur</t>
+  </si>
+  <si>
+    <t>Sur l'article sélectionné, clique sur le bouton supprimer</t>
+  </si>
+  <si>
+    <t>Dans cette page produit, l’utilisateur peut ajouter le produit à son panier via un bouton dédié si la couleur et la quantité rempli.</t>
+  </si>
+  <si>
+    <t>Couleur et quantité sélectionné, clique sur le bouton Ajout au panier</t>
+  </si>
+  <si>
+    <t>Dans cette page produit, si une couleur ou une quantité n'est pas sélectionné, un pop-up s'affiche</t>
+  </si>
+  <si>
+    <t>La couleur et la quantité n'est pas sélectionné par l'utilisateur</t>
+  </si>
+  <si>
+    <t>Un pop-up s'affiche pour indiquer a l'utilisateur de choisir une couleur et une quantité</t>
   </si>
 </sst>
 </file>
@@ -196,7 +212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -370,71 +386,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -469,18 +426,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -724,11 +669,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -736,267 +682,285 @@
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="3" width="58.44140625" customWidth="1"/>
     <col min="4" max="4" width="57.88671875" customWidth="1"/>
-    <col min="5" max="5" width="52.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+    </row>
+    <row r="4" spans="1:5" ht="108" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="86.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" ht="108" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="86.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" ht="86.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="64.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" ht="86.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>12</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="65.400000000000006" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
-        <v>13</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>40</v>
+      <c r="E18" s="12" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>